<commit_message>
UI cambiada y arreglados fallitos
</commit_message>
<xml_diff>
--- a/tableros/rapido.xlsx
+++ b/tableros/rapido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive - Universidade da Coruña\UDC4\TFG\ComunicELA-tfg\tableros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F870EF02-2B3A-46EE-8545-BA94F6633DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F27B537-6842-4B94-9238-E912ADBADCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>YO</t>
   </si>
   <si>
-    <t>QUIERO</t>
-  </si>
-  <si>
     <t>TU</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>BEBER</t>
+  </si>
+  <si>
+    <t>QUERER</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,13 +409,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -423,41 +423,41 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ponderaciones, modelo ajustado,  mas conjuntos, ajustable ponderacion en test
</commit_message>
<xml_diff>
--- a/tableros/rapido.xlsx
+++ b/tableros/rapido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive - Universidade da Coruña\UDC4\TFG\ComunicELA-tfg\tableros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F27B537-6842-4B94-9238-E912ADBADCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9622A-985A-4828-8C56-3E211F82290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="1530" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>TAB. INICIAL</t>
   </si>
@@ -73,6 +73,33 @@
   </si>
   <si>
     <t>QUERER</t>
+  </si>
+  <si>
+    <t>HOLA</t>
+  </si>
+  <si>
+    <t>ADIOS</t>
+  </si>
+  <si>
+    <t>QUE TAL ESTAS?</t>
+  </si>
+  <si>
+    <t>A MI</t>
+  </si>
+  <si>
+    <t>SABER</t>
+  </si>
+  <si>
+    <t>CONTAR</t>
+  </si>
+  <si>
+    <t>VIVIR</t>
+  </si>
+  <si>
+    <t>SENTIR</t>
+  </si>
+  <si>
+    <t>DECIR</t>
   </si>
 </sst>
 </file>
@@ -390,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,7 +431,7 @@
     <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +444,11 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -431,8 +461,11 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -445,8 +478,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -458,6 +494,26 @@
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>